<commit_message>
Pull request #97: oppdaterer kjentefeil excelfil fra 14. feb
Merge in SIR/skattemeldingen from kjente_feil_14 to master

Squashed commit of the following:

commit 7d5b568646a02f3ed805a4a481718fb506f0ecb0
Author: Martin Unhjem <>
Date:   Tue Feb 21 08:50:18 2023 +0100

    oppdaterer kjentefeil excelfil fra 14. feb
</commit_message>
<xml_diff>
--- a/docs/kjente feil/Kjente feil SME 2022.xlsx
+++ b/docs/kjente feil/Kjente feil SME 2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/k85256/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2FDFD54B-4BAF-8D40-A871-428B4970D1A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A3D06DC5-CDA5-4545-AEEE-91D9505D20BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="76040" yWindow="2680" windowWidth="29040" windowHeight="17640" xr2:uid="{F503ABD4-9C1D-4134-8421-54B31976295E}"/>
+    <workbookView xWindow="41200" yWindow="2580" windowWidth="29040" windowHeight="17640" xr2:uid="{F503ABD4-9C1D-4134-8421-54B31976295E}"/>
   </bookViews>
   <sheets>
     <sheet name="Kjente feil SME 2022" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
   <si>
     <t>Nr.</t>
   </si>
@@ -77,6 +77,15 @@
   </si>
   <si>
     <t>Skatteplikt</t>
+  </si>
+  <si>
+    <t>Etter å ha oppettet en instans av skattemelding i altinn kan man ikke oppdatere metadata på instansen (med for eksempel at signeres av revisor). Det må settes i den initielle opprettelsen. Det jobbes med feilfiks.</t>
+  </si>
+  <si>
+    <t>Altinn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">i informasjonsmodellen for FOU står det at 'Vedtak', 'AvgrensingIVedtak' at denne kan være 0 til mange. Dette er feil - det vil kun komme en forekomst her. Vi endrer ikke informasjonsmodellen for dette nå i år. Sender dere inn flere forekomster, som er lovlige iht XSD vil kun første forekomst faktisk bli sendt inn. </t>
   </si>
 </sst>
 </file>
@@ -759,7 +768,7 @@
   <dimension ref="A5:G53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -842,20 +851,50 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="1"/>
-      <c r="B8" s="2"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-    </row>
-    <row r="9" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="1"/>
-      <c r="B9" s="2"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
+      <c r="A8" s="1">
+        <v>3</v>
+      </c>
+      <c r="B8" s="2">
+        <v>44971</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>4</v>
+      </c>
+      <c r="B9" s="2">
+        <v>44971</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="10" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
@@ -1236,14 +1275,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="cac88abd-c5c8-440d-b517-c07797042b36" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4a745aa7-4b5a-438f-a0b7-deb914f75942">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1484,27 +1521,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="cac88abd-c5c8-440d-b517-c07797042b36" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4a745aa7-4b5a-438f-a0b7-deb914f75942">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70143F3C-BC9F-45A6-B9A2-5147BC76573E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51DF4BA9-15BA-4D1C-A9A8-6EA4D9ACD79B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="cac88abd-c5c8-440d-b517-c07797042b36"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="4a745aa7-4b5a-438f-a0b7-deb914f75942"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1529,9 +1559,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51DF4BA9-15BA-4D1C-A9A8-6EA4D9ACD79B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70143F3C-BC9F-45A6-B9A2-5147BC76573E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="cac88abd-c5c8-440d-b517-c07797042b36"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="4a745aa7-4b5a-438f-a0b7-deb914f75942"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>